<commit_message>
Updated BOM + .gitignore to ignore temporary DipTrace files
</commit_message>
<xml_diff>
--- a/pcb/export/bom/bom.xlsx
+++ b/pcb/export/bom/bom.xlsx
@@ -247,7 +247,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -262,6 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -610,7 +611,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -781,7 +782,7 @@
       <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E6">
@@ -800,7 +801,7 @@
         <v>0.17</v>
       </c>
       <c r="P6" s="2">
-        <f t="shared" ref="P6" si="0">K6*E6</f>
+        <f>K6*E6</f>
         <v>0.17</v>
       </c>
     </row>
@@ -814,7 +815,7 @@
       <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E7">
@@ -838,7 +839,7 @@
       <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="E8">
@@ -868,7 +869,7 @@
       <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E9">
@@ -891,7 +892,11 @@
         <v>0.35</v>
       </c>
     </row>
+    <row r="10" spans="1:16">
+      <c r="D10" s="10"/>
+    </row>
     <row r="11" spans="1:16">
+      <c r="D11" s="10"/>
       <c r="O11" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Added new potential switch to BOM
</commit_message>
<xml_diff>
--- a/pcb/export/bom/bom.xlsx
+++ b/pcb/export/bom/bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25280" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="bom.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>RefDes</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>418 121 270 808</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>Assembly</t>
   </si>
 </sst>
 </file>
@@ -230,10 +236,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -256,15 +268,15 @@
     <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="21">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -272,6 +284,9 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -279,6 +294,9 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -608,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -646,26 +664,26 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8" t="s">
+      <c r="I1" s="9"/>
+      <c r="J1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="9" t="s">
+      <c r="K1" s="9"/>
+      <c r="L1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9" t="s">
+      <c r="M1" s="10"/>
+      <c r="N1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="9"/>
+      <c r="O1" s="10"/>
       <c r="P1" t="s">
         <v>43</v>
       </c>
@@ -782,7 +800,7 @@
       <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E6">
@@ -815,7 +833,7 @@
       <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>16</v>
       </c>
       <c r="E7">
@@ -839,7 +857,7 @@
       <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>19</v>
       </c>
       <c r="E8">
@@ -869,7 +887,7 @@
       <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E9">
@@ -893,16 +911,46 @@
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="D10" s="10"/>
+      <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="D11" s="10"/>
-      <c r="O11" t="s">
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="P11" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="D15" s="8"/>
+      <c r="O15" t="s">
         <v>45</v>
       </c>
-      <c r="P11" s="2">
-        <f>SUM(P2:P10)</f>
-        <v>0.86899999999999999</v>
+      <c r="P15" s="2">
+        <f>SUM(P2:P13)</f>
+        <v>1.869</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added quick test functions, updated BOM, PCB CAD and drawings to reflect correct LED order. Did not update from v1.0 as this was a documentation error, not a design change.
</commit_message>
<xml_diff>
--- a/pcb/export/bom/bom.xlsx
+++ b/pcb/export/bom/bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>RefDes</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>Assembly</t>
+  </si>
+  <si>
+    <t>KaiFeng Electronics</t>
+  </si>
+  <si>
+    <t>KF-08P</t>
   </si>
 </sst>
 </file>
@@ -236,10 +242,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -269,14 +277,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -287,6 +295,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -297,6 +306,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -626,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -645,10 +655,10 @@
     <col min="9" max="9" width="14.33203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="14.33203125" style="3" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" style="1" customWidth="1"/>
-    <col min="12" max="15" width="14.33203125" customWidth="1"/>
+    <col min="12" max="17" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -664,31 +674,35 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="10"/>
+      <c r="H1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9" t="s">
+      <c r="I1" s="10"/>
+      <c r="J1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10" t="s">
+      <c r="K1" s="10"/>
+      <c r="L1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10" t="s">
+      <c r="M1" s="9"/>
+      <c r="N1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="10"/>
-      <c r="P1" t="s">
+      <c r="O1" s="9"/>
+      <c r="P1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="9"/>
+      <c r="R1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -707,17 +721,17 @@
       <c r="K2" s="5">
         <v>0.13</v>
       </c>
-      <c r="P2" s="2">
+      <c r="R2" s="2">
         <f>K2*E2</f>
         <v>0.13</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -729,17 +743,17 @@
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G3" s="5">
         <v>0.03</v>
       </c>
-      <c r="P3" s="2">
+      <c r="R3" s="2">
         <f>G3*E3</f>
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -761,17 +775,17 @@
       <c r="G4" s="5">
         <v>0.03</v>
       </c>
-      <c r="P4" s="2">
+      <c r="R4" s="2">
         <f>G4*E4</f>
         <v>0.03</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -783,17 +797,17 @@
         <v>1</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="5">
         <v>0.03</v>
       </c>
-      <c r="P5" s="2">
+      <c r="R5" s="2">
         <f>G5*E5</f>
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -818,12 +832,12 @@
       <c r="K6" s="5">
         <v>0.17</v>
       </c>
-      <c r="P6" s="2">
+      <c r="R6" s="2">
         <f>K6*E6</f>
         <v>0.17</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -845,12 +859,12 @@
       <c r="M7" s="7">
         <v>1.38E-2</v>
       </c>
-      <c r="P7" s="2">
+      <c r="R7" s="2">
         <f>M7*E7</f>
         <v>6.9000000000000006E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -875,12 +889,13 @@
       <c r="O8" s="1">
         <v>0.09</v>
       </c>
-      <c r="P8" s="2">
+      <c r="Q8" s="1"/>
+      <c r="R8" s="2">
         <f>G8*E8</f>
         <v>0.06</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -905,15 +920,18 @@
       <c r="I9" s="5">
         <v>0.35</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" t="s">
+        <v>50</v>
+      </c>
+      <c r="R9" s="2">
         <f>I9+K9*E9</f>
         <v>0.35</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:18">
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:18">
       <c r="C11" t="s">
         <v>47</v>
       </c>
@@ -921,14 +939,14 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="P11" s="2">
+      <c r="R11" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:18">
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:18">
       <c r="C13" t="s">
         <v>48</v>
       </c>
@@ -936,25 +954,29 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="P13" s="2">
+      <c r="R13" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:18">
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:18">
       <c r="D15" s="8"/>
       <c r="O15" t="s">
         <v>45</v>
       </c>
-      <c r="P15" s="2">
-        <f>SUM(P2:P13)</f>
+      <c r="Q15" t="s">
+        <v>45</v>
+      </c>
+      <c r="R15" s="2">
+        <f>SUM(R2:R13)</f>
         <v>1.869</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="P1:Q1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>

</xml_diff>